<commit_message>
quote out to quickturn
</commit_message>
<xml_diff>
--- a/hardware/permamote/rev_b/permamote_bom.xlsx
+++ b/hardware/permamote/rev_b/permamote_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="278">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">MANUFACTURER</t>
   </si>
   <si>
+    <t xml:space="preserve">MF</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOUSER</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t xml:space="preserve">0402_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C12, C13, C14, C15, C16, C17, C18, C19, C20</t>
+    <t xml:space="preserve">C13, C14, C15, C16, C17, C18, C19, C20, C21</t>
   </si>
   <si>
     <t xml:space="preserve">SMD Capacitor</t>
@@ -85,30 +88,6 @@
     <t xml:space="preserve">GRM155R71C104KA88J </t>
   </si>
   <si>
-    <t xml:space="preserve">0.5pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-6264-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM1555C1HR50WA01D </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-6269-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM1555C1HR80BA01D </t>
-  </si>
-  <si>
     <t xml:space="preserve">100M</t>
   </si>
   <si>
@@ -157,7 +136,7 @@
     <t xml:space="preserve">10nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C9, C10</t>
+    <t xml:space="preserve">C10, C11</t>
   </si>
   <si>
     <t xml:space="preserve">490-4516-1-ND</t>
@@ -175,7 +154,7 @@
     <t xml:space="preserve">0603_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C29, C30, C31</t>
+    <t xml:space="preserve">C30, C31, C32</t>
   </si>
   <si>
     <t xml:space="preserve">490-3896-1-ND</t>
@@ -229,10 +208,22 @@
     <t xml:space="preserve">HK100515NJ-T </t>
   </si>
   <si>
+    <t xml:space="preserve">1pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-1595-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL05C010CB5NNNC</t>
+  </si>
+  <si>
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C21, C22, C23, C24, C25</t>
+    <t xml:space="preserve">C22, C23, C24, C25, C26</t>
   </si>
   <si>
     <t xml:space="preserve">490-7195-1-ND </t>
@@ -274,28 +265,28 @@
     <t xml:space="preserve">732-3340-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3nH</t>
+    <t xml:space="preserve">3.9M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAG3301CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402JR-073M9L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9nH</t>
   </si>
   <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
-    <t xml:space="preserve">535-10426-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AISC-0402-3N3J-T </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.9M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAG3301CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402JR-073M9L</t>
+    <t xml:space="preserve">490-1131-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQP15MN3N9B02D</t>
   </si>
   <si>
     <t xml:space="preserve">32.768kHz</t>
@@ -364,7 +355,7 @@
     <t xml:space="preserve">4.7uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C26, C27, C28</t>
+    <t xml:space="preserve">C27, C28, C29</t>
   </si>
   <si>
     <t xml:space="preserve">445-5947-1-ND</t>
@@ -385,7 +376,7 @@
     <t xml:space="preserve">47nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C11</t>
+    <t xml:space="preserve">C12</t>
   </si>
   <si>
     <t xml:space="preserve">445-1264-1-ND</t>
@@ -454,6 +445,18 @@
     <t xml:space="preserve">RC0603FR-0780K6L </t>
   </si>
   <si>
+    <t xml:space="preserve">820pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-6535-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL05B821KO5NNNC</t>
+  </si>
+  <si>
     <t xml:space="preserve">9.1M</t>
   </si>
   <si>
@@ -532,7 +535,7 @@
     <t xml:space="preserve">BAT-HLD-001-THM</t>
   </si>
   <si>
-    <t xml:space="preserve">Do Not Populate</t>
+    <t xml:space="preserve">DNP</t>
   </si>
   <si>
     <t xml:space="preserve">BAT_PACKCR123A</t>
@@ -574,10 +577,7 @@
     <t xml:space="preserve">BQ25505RGRR</t>
   </si>
   <si>
-    <t xml:space="preserve">DNP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C32, C33</t>
+    <t xml:space="preserve">C33, C34</t>
   </si>
   <si>
     <t xml:space="preserve">R6, R7</t>
@@ -927,8 +927,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -949,26 +953,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="36.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="134.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="33.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,57 +1019,60 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,25 +1080,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,129 +1106,129 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="0" t="s">
         <v>39</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,103 +1236,106 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G10" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="0" t="s">
         <v>68</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,28 +1343,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>74437324220</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>74437324220</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,25 +1369,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>74437324220</v>
+        <v>23</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>82</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>74437324220</v>
+      <c r="K15" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,25 +1395,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J16" s="0" t="s">
         <v>87</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,25 +1421,28 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,28 +1450,28 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,106 +1479,103 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="J20" s="0" t="s">
         <v>112</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>113</v>
+      <c r="B21" s="0" t="n">
+        <v>470</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>114</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="K21" s="0" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>470</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>117</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J22" s="0" t="s">
         <v>119</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,25 +1583,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="J23" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,25 +1609,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" s="0" t="s">
         <v>127</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,25 +1635,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25" s="0" t="s">
         <v>131</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,25 +1661,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="J26" s="0" t="s">
         <v>135</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,25 +1687,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="J27" s="0" t="s">
         <v>139</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,25 +1713,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="J28" s="0" t="s">
         <v>143</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,25 +1739,25 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="J29" s="0" t="s">
         <v>147</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,28 +1765,28 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,28 +1794,28 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="J31" s="0" t="s">
         <v>158</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,28 +1823,28 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E32" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,31 +1852,31 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="I33" s="0" t="s">
         <v>168</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="N33" s="0" t="s">
+      <c r="K33" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,28 +1884,31 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="O34" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,28 +1916,28 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="J35" s="0" t="s">
         <v>183</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,22 +1945,22 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>185</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="N36" s="0" t="s">
-        <v>170</v>
+        <v>19</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,28 +1968,28 @@
         <v>2</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>186</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N37" s="0" t="s">
-        <v>170</v>
+        <v>35</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,7 +2017,7 @@
       <c r="H38" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="K38" s="0" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2032,7 +2043,7 @@
       <c r="G39" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="K39" s="0" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2055,13 +2066,13 @@
       <c r="F40" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="K40" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="L40" s="0" t="n">
+      <c r="M40" s="0" t="n">
         <v>1146033</v>
       </c>
-      <c r="M40" s="0" t="s">
+      <c r="N40" s="0" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2087,10 +2098,10 @@
       <c r="H41" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="J41" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="K41" s="0" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2110,8 +2121,8 @@
       <c r="E42" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="N42" s="0" t="s">
-        <v>170</v>
+      <c r="O42" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,7 +2150,7 @@
       <c r="H43" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="K43" s="0" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2168,7 +2179,7 @@
       <c r="H44" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="K44" s="0" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2194,13 +2205,13 @@
       <c r="G45" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="J45" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="J45" s="0" t="s">
+      <c r="K45" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="K45" s="0" t="s">
+      <c r="L45" s="0" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2229,7 +2240,7 @@
       <c r="H46" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="K46" s="0" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2258,7 +2269,7 @@
       <c r="H47" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="K47" s="0" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2287,7 +2298,7 @@
       <c r="H48" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="J48" s="0" t="s">
+      <c r="K48" s="0" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2313,10 +2324,10 @@
       <c r="G49" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="J49" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="J49" s="0" t="s">
+      <c r="K49" s="0" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2345,7 +2356,7 @@
       <c r="H50" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="J50" s="0" t="s">
+      <c r="K50" s="0" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2371,11 +2382,11 @@
       <c r="G51" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="K51" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="N51" s="0" t="s">
-        <v>170</v>
+      <c r="O51" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2411,7 @@
       <c r="G52" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="J52" s="0" t="s">
+      <c r="K52" s="0" t="s">
         <v>277</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add part marker to U12
</commit_message>
<xml_diff>
--- a/hardware/permamote/rev_b/permamote_bom.xlsx
+++ b/hardware/permamote/rev_b/permamote_bom.xlsx
@@ -103,10 +103,10 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">541-100MAHCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMC0402JT100M </t>
+    <t xml:space="preserve">HMC0402JT100MCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMC0402JT100M</t>
   </si>
   <si>
     <t xml:space="preserve">100pF</t>
@@ -868,6 +868,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -956,7 +957,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -964,7 +965,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="36.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="134.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.21"/>

</xml_diff>